<commit_message>
Set new default testings
</commit_message>
<xml_diff>
--- a/randomPlanarGraph/data/FFP_n15_no1.xlsx
+++ b/randomPlanarGraph/data/FFP_n15_no1.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,16 +470,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D2" t="n">
-        <v>392.5620969986787</v>
+        <v>309.6126612398143</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -487,16 +487,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>392.5620969986787</v>
+        <v>309.6126612398143</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -504,16 +504,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>282.4606167238187</v>
+        <v>79.02531240052139</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -521,16 +521,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>282.4606167238187</v>
+        <v>79.02531240052139</v>
       </c>
       <c r="E5" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>216.529443725328</v>
+        <v>113.6353818139403</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -555,16 +555,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>216.529443725328</v>
+        <v>113.6353818139403</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -572,16 +572,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" t="n">
-        <v>389.8820334408858</v>
+        <v>178.4040358287895</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -589,16 +589,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>389.8820334408858</v>
+        <v>178.4040358287895</v>
       </c>
       <c r="E9" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -606,16 +606,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" t="n">
-        <v>438.0559325017754</v>
+        <v>362.7740343519641</v>
       </c>
       <c r="E10" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -623,16 +623,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>438.0559325017754</v>
+        <v>362.7740343519641</v>
       </c>
       <c r="E11" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -640,16 +640,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D12" t="n">
-        <v>234.292552165023</v>
+        <v>71.58910531638176</v>
       </c>
       <c r="E12" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -657,16 +657,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C13" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>234.292552165023</v>
+        <v>71.58910531638176</v>
       </c>
       <c r="E13" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
@@ -674,16 +674,16 @@
         <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>262.5509474368737</v>
+        <v>242.9423799998675</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
@@ -691,16 +691,16 @@
         <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>262.5509474368737</v>
+        <v>242.9423799998675</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
@@ -708,16 +708,16 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C16" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>110.4536101718726</v>
+        <v>237.1919054268083</v>
       </c>
       <c r="E16" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -725,16 +725,16 @@
         <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C17" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D17" t="n">
-        <v>110.4536101718726</v>
+        <v>237.1919054268083</v>
       </c>
       <c r="E17" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -742,16 +742,16 @@
         <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C18" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D18" t="n">
-        <v>233.1179958733345</v>
+        <v>300.273208928136</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
@@ -759,16 +759,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D19" t="n">
-        <v>233.1179958733345</v>
+        <v>300.273208928136</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
@@ -776,16 +776,16 @@
         <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C20" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D20" t="n">
-        <v>215.7452201092761</v>
+        <v>351.7570184090148</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
@@ -793,16 +793,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D21" t="n">
-        <v>215.7452201092761</v>
+        <v>351.7570184090148</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22">
@@ -810,16 +810,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D22" t="n">
-        <v>48.66210024238575</v>
+        <v>351.9232870953555</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -827,16 +827,16 @@
         <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>48.66210024238575</v>
+        <v>351.9232870953555</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
@@ -844,16 +844,16 @@
         <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D24" t="n">
-        <v>80.95677859203639</v>
+        <v>314.4137401577736</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
@@ -861,16 +861,16 @@
         <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D25" t="n">
-        <v>80.95677859203639</v>
+        <v>314.4137401577736</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
@@ -878,16 +878,16 @@
         <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C26" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D26" t="n">
-        <v>320.1312230945304</v>
+        <v>186.2713075060139</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -895,16 +895,16 @@
         <v>1</v>
       </c>
       <c r="B27" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C27" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D27" t="n">
-        <v>320.1312230945304</v>
+        <v>186.2713075060139</v>
       </c>
       <c r="E27" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
@@ -915,13 +915,13 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D28" t="n">
-        <v>311.0884118703235</v>
+        <v>176.3235662071295</v>
       </c>
       <c r="E28" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
@@ -929,16 +929,16 @@
         <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C29" t="n">
         <v>6</v>
       </c>
       <c r="D29" t="n">
-        <v>311.0884118703235</v>
+        <v>176.3235662071295</v>
       </c>
       <c r="E29" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
@@ -946,16 +946,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C30" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D30" t="n">
-        <v>503.5642957954823</v>
+        <v>754.443503517659</v>
       </c>
       <c r="E30" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31">
@@ -963,16 +963,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C31" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D31" t="n">
-        <v>503.5642957954823</v>
+        <v>754.443503517659</v>
       </c>
       <c r="E31" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32">
@@ -980,16 +980,16 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C32" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D32" t="n">
-        <v>124.9519907804594</v>
+        <v>45.5411901469428</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
@@ -997,16 +997,16 @@
         <v>1</v>
       </c>
       <c r="B33" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C33" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D33" t="n">
-        <v>124.9519907804594</v>
+        <v>45.5411901469428</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
@@ -1017,13 +1017,13 @@
         <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D34" t="n">
-        <v>232.4220299369231</v>
+        <v>567.6310421391698</v>
       </c>
       <c r="E34" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35">
@@ -1031,16 +1031,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C35" t="n">
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>232.4220299369231</v>
+        <v>567.6310421391698</v>
       </c>
       <c r="E35" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36">
@@ -1048,16 +1048,16 @@
         <v>1</v>
       </c>
       <c r="B36" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" t="n">
         <v>9</v>
       </c>
-      <c r="C36" t="n">
-        <v>15</v>
-      </c>
       <c r="D36" t="n">
-        <v>88.05679985100527</v>
+        <v>342.4981751776205</v>
       </c>
       <c r="E36" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37">
@@ -1065,16 +1065,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C37" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D37" t="n">
-        <v>88.05679985100527</v>
+        <v>342.4981751776205</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38">
@@ -1085,13 +1085,13 @@
         <v>2</v>
       </c>
       <c r="C38" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D38" t="n">
-        <v>197.8736970898356</v>
+        <v>203.5534327885433</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39">
@@ -1099,16 +1099,16 @@
         <v>1</v>
       </c>
       <c r="B39" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C39" t="n">
         <v>2</v>
       </c>
       <c r="D39" t="n">
-        <v>197.8736970898356</v>
+        <v>203.5534327885433</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40">
@@ -1116,16 +1116,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C40" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D40" t="n">
-        <v>693.9510069161944</v>
+        <v>64.19501538281614</v>
       </c>
       <c r="E40" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
@@ -1133,16 +1133,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C41" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41" t="n">
-        <v>693.9510069161944</v>
+        <v>64.19501538281614</v>
       </c>
       <c r="E41" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -1150,13 +1150,13 @@
         <v>1</v>
       </c>
       <c r="B42" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C42" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D42" t="n">
-        <v>155.183762037141</v>
+        <v>146.6594695203825</v>
       </c>
       <c r="E42" t="n">
         <v>10</v>
@@ -1167,13 +1167,13 @@
         <v>1</v>
       </c>
       <c r="B43" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C43" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D43" t="n">
-        <v>155.183762037141</v>
+        <v>146.6594695203825</v>
       </c>
       <c r="E43" t="n">
         <v>10</v>
@@ -1184,16 +1184,16 @@
         <v>1</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C44" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D44" t="n">
-        <v>339.2005306599623</v>
+        <v>497.3469613861132</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45">
@@ -1201,16 +1201,16 @@
         <v>1</v>
       </c>
       <c r="B45" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D45" t="n">
-        <v>339.2005306599623</v>
+        <v>497.3469613861132</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46">
@@ -1218,16 +1218,16 @@
         <v>1</v>
       </c>
       <c r="B46" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C46" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D46" t="n">
-        <v>185.7848217697022</v>
+        <v>623.0393246015857</v>
       </c>
       <c r="E46" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47">
@@ -1235,16 +1235,16 @@
         <v>1</v>
       </c>
       <c r="B47" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C47" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D47" t="n">
-        <v>185.7848217697022</v>
+        <v>623.0393246015857</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48">
@@ -1252,16 +1252,16 @@
         <v>1</v>
       </c>
       <c r="B48" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C48" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D48" t="n">
-        <v>310.7104761671225</v>
+        <v>187.2591786802452</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49">
@@ -1269,16 +1269,16 @@
         <v>1</v>
       </c>
       <c r="B49" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>310.7104761671225</v>
+        <v>187.2591786802452</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50">
@@ -1286,16 +1286,16 @@
         <v>1</v>
       </c>
       <c r="B50" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C50" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D50" t="n">
-        <v>163.6245702820943</v>
+        <v>62.96824596572466</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51">
@@ -1303,16 +1303,16 @@
         <v>1</v>
       </c>
       <c r="B51" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C51" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D51" t="n">
-        <v>163.6245702820943</v>
+        <v>62.96824596572466</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52">
@@ -1320,16 +1320,16 @@
         <v>1</v>
       </c>
       <c r="B52" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D52" t="n">
-        <v>41.4004830889689</v>
+        <v>43.01162633521314</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
@@ -1337,16 +1337,16 @@
         <v>1</v>
       </c>
       <c r="B53" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C53" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>41.4004830889689</v>
+        <v>43.01162633521314</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54">
@@ -1354,16 +1354,16 @@
         <v>1</v>
       </c>
       <c r="B54" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C54" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D54" t="n">
-        <v>415.7811924558397</v>
+        <v>109.3846424321074</v>
       </c>
       <c r="E54" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55">
@@ -1371,16 +1371,16 @@
         <v>1</v>
       </c>
       <c r="B55" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C55" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D55" t="n">
-        <v>415.7811924558397</v>
+        <v>109.3846424321074</v>
       </c>
       <c r="E55" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56">
@@ -1388,13 +1388,13 @@
         <v>1</v>
       </c>
       <c r="B56" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C56" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D56" t="n">
-        <v>190.2445794234359</v>
+        <v>66.40783086353596</v>
       </c>
       <c r="E56" t="n">
         <v>5</v>
@@ -1405,13 +1405,13 @@
         <v>1</v>
       </c>
       <c r="B57" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C57" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D57" t="n">
-        <v>190.2445794234359</v>
+        <v>66.40783086353596</v>
       </c>
       <c r="E57" t="n">
         <v>5</v>
@@ -1422,16 +1422,16 @@
         <v>1</v>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C58" t="n">
         <v>7</v>
       </c>
       <c r="D58" t="n">
-        <v>228.3549868078208</v>
+        <v>90.04998611882181</v>
       </c>
       <c r="E58" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59">
@@ -1442,13 +1442,13 @@
         <v>7</v>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D59" t="n">
-        <v>228.3549868078208</v>
+        <v>90.04998611882181</v>
       </c>
       <c r="E59" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60">
@@ -1456,16 +1456,16 @@
         <v>1</v>
       </c>
       <c r="B60" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C60" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D60" t="n">
-        <v>216.9469981354893</v>
+        <v>208.4346420343797</v>
       </c>
       <c r="E60" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61">
@@ -1473,50 +1473,50 @@
         <v>1</v>
       </c>
       <c r="B61" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D61" t="n">
-        <v>216.9469981354893</v>
+        <v>208.4346420343797</v>
       </c>
       <c r="E61" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C62" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D62" t="n">
-        <v>274.2207140243056</v>
+        <v>309.6126612398143</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B63" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C63" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D63" t="n">
-        <v>274.2207140243056</v>
+        <v>309.6126612398143</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64">
@@ -1524,16 +1524,16 @@
         <v>2</v>
       </c>
       <c r="B64" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D64" t="n">
-        <v>392.5620969986787</v>
+        <v>79.02531240052139</v>
       </c>
       <c r="E64" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65">
@@ -1541,16 +1541,16 @@
         <v>2</v>
       </c>
       <c r="B65" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C65" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D65" t="n">
-        <v>392.5620969986787</v>
+        <v>79.02531240052139</v>
       </c>
       <c r="E65" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66">
@@ -1558,16 +1558,16 @@
         <v>2</v>
       </c>
       <c r="B66" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C66" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D66" t="n">
-        <v>282.4606167238187</v>
+        <v>113.6353818139403</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67">
@@ -1575,16 +1575,16 @@
         <v>2</v>
       </c>
       <c r="B67" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C67" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D67" t="n">
-        <v>282.4606167238187</v>
+        <v>113.6353818139403</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68">
@@ -1592,16 +1592,16 @@
         <v>2</v>
       </c>
       <c r="B68" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C68" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D68" t="n">
-        <v>216.529443725328</v>
+        <v>178.4040358287895</v>
       </c>
       <c r="E68" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
@@ -1609,16 +1609,16 @@
         <v>2</v>
       </c>
       <c r="B69" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C69" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D69" t="n">
-        <v>216.529443725328</v>
+        <v>178.4040358287895</v>
       </c>
       <c r="E69" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70">
@@ -1626,16 +1626,16 @@
         <v>2</v>
       </c>
       <c r="B70" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C70" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D70" t="n">
-        <v>389.8820334408858</v>
+        <v>362.7740343519641</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71">
@@ -1643,16 +1643,16 @@
         <v>2</v>
       </c>
       <c r="B71" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C71" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D71" t="n">
-        <v>389.8820334408858</v>
+        <v>362.7740343519641</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72">
@@ -1660,16 +1660,16 @@
         <v>2</v>
       </c>
       <c r="B72" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C72" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D72" t="n">
-        <v>438.0559325017754</v>
+        <v>71.58910531638176</v>
       </c>
       <c r="E72" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73">
@@ -1677,16 +1677,16 @@
         <v>2</v>
       </c>
       <c r="B73" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C73" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D73" t="n">
-        <v>438.0559325017754</v>
+        <v>71.58910531638176</v>
       </c>
       <c r="E73" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74">
@@ -1694,16 +1694,16 @@
         <v>2</v>
       </c>
       <c r="B74" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C74" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D74" t="n">
-        <v>234.292552165023</v>
+        <v>242.9423799998675</v>
       </c>
       <c r="E74" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75">
@@ -1711,16 +1711,16 @@
         <v>2</v>
       </c>
       <c r="B75" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C75" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D75" t="n">
-        <v>234.292552165023</v>
+        <v>242.9423799998675</v>
       </c>
       <c r="E75" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76">
@@ -1728,16 +1728,16 @@
         <v>2</v>
       </c>
       <c r="B76" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C76" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D76" t="n">
-        <v>262.5509474368737</v>
+        <v>237.1919054268083</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77">
@@ -1745,16 +1745,16 @@
         <v>2</v>
       </c>
       <c r="B77" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D77" t="n">
-        <v>262.5509474368737</v>
+        <v>237.1919054268083</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78">
@@ -1762,16 +1762,16 @@
         <v>2</v>
       </c>
       <c r="B78" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C78" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D78" t="n">
-        <v>110.4536101718726</v>
+        <v>300.273208928136</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79">
@@ -1779,16 +1779,16 @@
         <v>2</v>
       </c>
       <c r="B79" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C79" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D79" t="n">
-        <v>110.4536101718726</v>
+        <v>300.273208928136</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80">
@@ -1796,16 +1796,16 @@
         <v>2</v>
       </c>
       <c r="B80" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C80" t="n">
         <v>15</v>
       </c>
       <c r="D80" t="n">
-        <v>233.1179958733345</v>
+        <v>351.7570184090148</v>
       </c>
       <c r="E80" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81">
@@ -1816,13 +1816,13 @@
         <v>15</v>
       </c>
       <c r="C81" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D81" t="n">
-        <v>233.1179958733345</v>
+        <v>351.7570184090148</v>
       </c>
       <c r="E81" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82">
@@ -1830,16 +1830,16 @@
         <v>2</v>
       </c>
       <c r="B82" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C82" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D82" t="n">
-        <v>215.7452201092761</v>
+        <v>351.9232870953555</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83">
@@ -1847,16 +1847,16 @@
         <v>2</v>
       </c>
       <c r="B83" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D83" t="n">
-        <v>215.7452201092761</v>
+        <v>351.9232870953555</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84">
@@ -1864,16 +1864,16 @@
         <v>2</v>
       </c>
       <c r="B84" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C84" t="n">
         <v>9</v>
       </c>
       <c r="D84" t="n">
-        <v>48.66210024238575</v>
+        <v>314.4137401577736</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85">
@@ -1884,13 +1884,13 @@
         <v>9</v>
       </c>
       <c r="C85" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D85" t="n">
-        <v>48.66210024238575</v>
+        <v>314.4137401577736</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86">
@@ -1898,16 +1898,16 @@
         <v>2</v>
       </c>
       <c r="B86" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C86" t="n">
         <v>15</v>
       </c>
       <c r="D86" t="n">
-        <v>80.95677859203639</v>
+        <v>186.2713075060139</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87">
@@ -1918,13 +1918,13 @@
         <v>15</v>
       </c>
       <c r="C87" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D87" t="n">
-        <v>80.95677859203639</v>
+        <v>186.2713075060139</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88">
@@ -1932,16 +1932,16 @@
         <v>2</v>
       </c>
       <c r="B88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C88" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D88" t="n">
-        <v>320.1312230945304</v>
+        <v>176.3235662071295</v>
       </c>
       <c r="E88" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89">
@@ -1949,16 +1949,16 @@
         <v>2</v>
       </c>
       <c r="B89" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D89" t="n">
-        <v>320.1312230945304</v>
+        <v>176.3235662071295</v>
       </c>
       <c r="E89" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90">
@@ -1966,16 +1966,16 @@
         <v>2</v>
       </c>
       <c r="B90" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C90" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D90" t="n">
-        <v>311.0884118703235</v>
+        <v>754.443503517659</v>
       </c>
       <c r="E90" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91">
@@ -1983,16 +1983,16 @@
         <v>2</v>
       </c>
       <c r="B91" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C91" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D91" t="n">
-        <v>311.0884118703235</v>
+        <v>754.443503517659</v>
       </c>
       <c r="E91" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92">
@@ -2000,16 +2000,16 @@
         <v>2</v>
       </c>
       <c r="B92" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C92" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D92" t="n">
-        <v>503.5642957954823</v>
+        <v>45.5411901469428</v>
       </c>
       <c r="E92" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93">
@@ -2017,16 +2017,16 @@
         <v>2</v>
       </c>
       <c r="B93" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C93" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D93" t="n">
-        <v>503.5642957954823</v>
+        <v>45.5411901469428</v>
       </c>
       <c r="E93" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94">
@@ -2034,16 +2034,16 @@
         <v>2</v>
       </c>
       <c r="B94" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C94" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D94" t="n">
-        <v>124.9519907804594</v>
+        <v>567.6310421391698</v>
       </c>
       <c r="E94" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="95">
@@ -2051,16 +2051,16 @@
         <v>2</v>
       </c>
       <c r="B95" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C95" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D95" t="n">
-        <v>124.9519907804594</v>
+        <v>567.6310421391698</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96">
@@ -2068,16 +2068,16 @@
         <v>2</v>
       </c>
       <c r="B96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C96" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D96" t="n">
-        <v>232.4220299369231</v>
+        <v>342.4981751776205</v>
       </c>
       <c r="E96" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97">
@@ -2085,16 +2085,16 @@
         <v>2</v>
       </c>
       <c r="B97" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D97" t="n">
-        <v>232.4220299369231</v>
+        <v>342.4981751776205</v>
       </c>
       <c r="E97" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98">
@@ -2102,16 +2102,16 @@
         <v>2</v>
       </c>
       <c r="B98" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C98" t="n">
         <v>15</v>
       </c>
       <c r="D98" t="n">
-        <v>88.05679985100527</v>
+        <v>203.5534327885433</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99">
@@ -2122,13 +2122,13 @@
         <v>15</v>
       </c>
       <c r="C99" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D99" t="n">
-        <v>88.05679985100527</v>
+        <v>203.5534327885433</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100">
@@ -2136,16 +2136,16 @@
         <v>2</v>
       </c>
       <c r="B100" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C100" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D100" t="n">
-        <v>197.8736970898356</v>
+        <v>64.19501538281614</v>
       </c>
       <c r="E100" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101">
@@ -2153,16 +2153,16 @@
         <v>2</v>
       </c>
       <c r="B101" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C101" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D101" t="n">
-        <v>197.8736970898356</v>
+        <v>64.19501538281614</v>
       </c>
       <c r="E101" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102">
@@ -2170,16 +2170,16 @@
         <v>2</v>
       </c>
       <c r="B102" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C102" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D102" t="n">
-        <v>693.9510069161944</v>
+        <v>146.6594695203825</v>
       </c>
       <c r="E102" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103">
@@ -2187,16 +2187,16 @@
         <v>2</v>
       </c>
       <c r="B103" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C103" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D103" t="n">
-        <v>693.9510069161944</v>
+        <v>146.6594695203825</v>
       </c>
       <c r="E103" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104">
@@ -2204,16 +2204,16 @@
         <v>2</v>
       </c>
       <c r="B104" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C104" t="n">
         <v>12</v>
       </c>
       <c r="D104" t="n">
-        <v>155.183762037141</v>
+        <v>497.3469613861132</v>
       </c>
       <c r="E104" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="105">
@@ -2224,13 +2224,13 @@
         <v>12</v>
       </c>
       <c r="C105" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D105" t="n">
-        <v>155.183762037141</v>
+        <v>497.3469613861132</v>
       </c>
       <c r="E105" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106">
@@ -2238,16 +2238,16 @@
         <v>2</v>
       </c>
       <c r="B106" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C106" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D106" t="n">
-        <v>339.2005306599623</v>
+        <v>623.0393246015857</v>
       </c>
       <c r="E106" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="107">
@@ -2255,16 +2255,16 @@
         <v>2</v>
       </c>
       <c r="B107" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D107" t="n">
-        <v>339.2005306599623</v>
+        <v>623.0393246015857</v>
       </c>
       <c r="E107" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="108">
@@ -2272,16 +2272,16 @@
         <v>2</v>
       </c>
       <c r="B108" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C108" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D108" t="n">
-        <v>185.7848217697022</v>
+        <v>187.2591786802452</v>
       </c>
       <c r="E108" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109">
@@ -2289,16 +2289,16 @@
         <v>2</v>
       </c>
       <c r="B109" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C109" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D109" t="n">
-        <v>185.7848217697022</v>
+        <v>187.2591786802452</v>
       </c>
       <c r="E109" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110">
@@ -2306,16 +2306,16 @@
         <v>2</v>
       </c>
       <c r="B110" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C110" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D110" t="n">
-        <v>310.7104761671225</v>
+        <v>62.96824596572466</v>
       </c>
       <c r="E110" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111">
@@ -2323,16 +2323,16 @@
         <v>2</v>
       </c>
       <c r="B111" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C111" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D111" t="n">
-        <v>310.7104761671225</v>
+        <v>62.96824596572466</v>
       </c>
       <c r="E111" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112">
@@ -2340,16 +2340,16 @@
         <v>2</v>
       </c>
       <c r="B112" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C112" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D112" t="n">
-        <v>163.6245702820943</v>
+        <v>43.01162633521314</v>
       </c>
       <c r="E112" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113">
@@ -2357,16 +2357,16 @@
         <v>2</v>
       </c>
       <c r="B113" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C113" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D113" t="n">
-        <v>163.6245702820943</v>
+        <v>43.01162633521314</v>
       </c>
       <c r="E113" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114">
@@ -2374,16 +2374,16 @@
         <v>2</v>
       </c>
       <c r="B114" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C114" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D114" t="n">
-        <v>41.4004830889689</v>
+        <v>109.3846424321074</v>
       </c>
       <c r="E114" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115">
@@ -2391,16 +2391,16 @@
         <v>2</v>
       </c>
       <c r="B115" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C115" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D115" t="n">
-        <v>41.4004830889689</v>
+        <v>109.3846424321074</v>
       </c>
       <c r="E115" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116">
@@ -2408,16 +2408,16 @@
         <v>2</v>
       </c>
       <c r="B116" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C116" t="n">
         <v>14</v>
       </c>
       <c r="D116" t="n">
-        <v>415.7811924558397</v>
+        <v>66.40783086353596</v>
       </c>
       <c r="E116" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117">
@@ -2428,13 +2428,13 @@
         <v>14</v>
       </c>
       <c r="C117" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D117" t="n">
-        <v>415.7811924558397</v>
+        <v>66.40783086353596</v>
       </c>
       <c r="E117" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118">
@@ -2442,16 +2442,16 @@
         <v>2</v>
       </c>
       <c r="B118" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C118" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D118" t="n">
-        <v>190.2445794234359</v>
+        <v>90.04998611882181</v>
       </c>
       <c r="E118" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119">
@@ -2459,16 +2459,16 @@
         <v>2</v>
       </c>
       <c r="B119" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C119" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D119" t="n">
-        <v>190.2445794234359</v>
+        <v>90.04998611882181</v>
       </c>
       <c r="E119" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="120">
@@ -2476,16 +2476,16 @@
         <v>2</v>
       </c>
       <c r="B120" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C120" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D120" t="n">
-        <v>228.3549868078208</v>
+        <v>208.4346420343797</v>
       </c>
       <c r="E120" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121">
@@ -2493,84 +2493,16 @@
         <v>2</v>
       </c>
       <c r="B121" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C121" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D121" t="n">
-        <v>228.3549868078208</v>
+        <v>208.4346420343797</v>
       </c>
       <c r="E121" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n">
-        <v>2</v>
-      </c>
-      <c r="B122" t="n">
-        <v>1</v>
-      </c>
-      <c r="C122" t="n">
-        <v>13</v>
-      </c>
-      <c r="D122" t="n">
-        <v>216.9469981354893</v>
-      </c>
-      <c r="E122" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="n">
-        <v>2</v>
-      </c>
-      <c r="B123" t="n">
-        <v>13</v>
-      </c>
-      <c r="C123" t="n">
-        <v>1</v>
-      </c>
-      <c r="D123" t="n">
-        <v>216.9469981354893</v>
-      </c>
-      <c r="E123" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="n">
-        <v>2</v>
-      </c>
-      <c r="B124" t="n">
-        <v>3</v>
-      </c>
-      <c r="C124" t="n">
-        <v>10</v>
-      </c>
-      <c r="D124" t="n">
-        <v>274.2207140243056</v>
-      </c>
-      <c r="E124" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="n">
-        <v>2</v>
-      </c>
-      <c r="B125" t="n">
-        <v>10</v>
-      </c>
-      <c r="C125" t="n">
-        <v>3</v>
-      </c>
-      <c r="D125" t="n">
-        <v>274.2207140243056</v>
-      </c>
-      <c r="E125" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2621,33 +2553,33 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>510</v>
+        <v>867</v>
       </c>
       <c r="B2" t="n">
-        <v>268</v>
+        <v>512</v>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B3" t="n">
-        <v>126</v>
+        <v>406</v>
       </c>
       <c r="C3" t="n">
         <v>15</v>
       </c>
       <c r="D3" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
         <v>5</v>
@@ -2655,16 +2587,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>203</v>
+        <v>946</v>
       </c>
       <c r="B4" t="n">
-        <v>281</v>
+        <v>514</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
         <v>3</v>
@@ -2672,135 +2604,135 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1152</v>
+        <v>401</v>
       </c>
       <c r="B5" t="n">
-        <v>532</v>
+        <v>228</v>
       </c>
       <c r="C5" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>949</v>
+        <v>344</v>
       </c>
       <c r="B6" t="n">
-        <v>196</v>
+        <v>347</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>332</v>
+        <v>733</v>
       </c>
       <c r="B7" t="n">
-        <v>461</v>
+        <v>144</v>
       </c>
       <c r="C7" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
         <v>8</v>
-      </c>
-      <c r="E7" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>735</v>
+        <v>868</v>
       </c>
       <c r="B8" t="n">
-        <v>229</v>
+        <v>469</v>
       </c>
       <c r="C8" t="n">
         <v>15</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1102</v>
+        <v>991</v>
       </c>
       <c r="B9" t="n">
-        <v>254</v>
+        <v>521</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>195</v>
+        <v>110</v>
       </c>
       <c r="B10" t="n">
-        <v>329</v>
+        <v>137</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>22</v>
+        <v>1052</v>
       </c>
       <c r="B11" t="n">
-        <v>487</v>
+        <v>541</v>
       </c>
       <c r="C11" t="n">
         <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>276</v>
+        <v>685</v>
       </c>
       <c r="B12" t="n">
-        <v>21</v>
+        <v>247</v>
       </c>
       <c r="C12" t="n">
         <v>5</v>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
         <v>2</v>
@@ -2808,16 +2740,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>465</v>
+        <v>1160</v>
       </c>
       <c r="B13" t="n">
-        <v>57</v>
+        <v>399</v>
       </c>
       <c r="C13" t="n">
         <v>5</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E13" t="n">
         <v>7</v>
@@ -2825,53 +2757,53 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>305</v>
+        <v>622</v>
       </c>
       <c r="B14" t="n">
-        <v>339</v>
+        <v>281</v>
       </c>
       <c r="C14" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>714</v>
+        <v>301</v>
       </c>
       <c r="B15" t="n">
-        <v>539</v>
+        <v>469</v>
       </c>
       <c r="C15" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>280</v>
+        <v>525</v>
       </c>
       <c r="B16" t="n">
-        <v>306</v>
+        <v>391</v>
       </c>
       <c r="C16" t="n">
         <v>10</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2907,7 +2839,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>2</v>
@@ -2915,7 +2847,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>5</v>
@@ -2949,7 +2881,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3026,30 +2958,30 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>392.5620969986787</v>
+        <v>309.6126612398143</v>
       </c>
       <c r="D2" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>392.5620969986787</v>
+        <v>309.6126612398143</v>
       </c>
       <c r="D3" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -3057,153 +2989,153 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>282.4606167238187</v>
+        <v>131.9469590403659</v>
       </c>
       <c r="D4" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>282.4606167238187</v>
+        <v>131.9469590403659</v>
       </c>
       <c r="D5" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>216.529443725328</v>
+        <v>113.6353818139403</v>
       </c>
       <c r="D6" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>216.529443725328</v>
+        <v>113.6353818139403</v>
       </c>
       <c r="D7" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
-        <v>438.0559325017754</v>
+        <v>178.4040358287895</v>
       </c>
       <c r="D8" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>438.0559325017754</v>
+        <v>178.4040358287895</v>
       </c>
       <c r="D9" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>234.292552165023</v>
+        <v>71.58910531638176</v>
       </c>
       <c r="D10" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>234.292552165023</v>
+        <v>71.58910531638176</v>
       </c>
       <c r="D11" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B12" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="n">
-        <v>110.4536101718726</v>
+        <v>242.9423799998675</v>
       </c>
       <c r="D12" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>110.4536101718726</v>
+        <v>242.9423799998675</v>
       </c>
       <c r="D13" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B14" t="n">
         <v>15</v>
       </c>
       <c r="C14" t="n">
-        <v>233.1179958733345</v>
+        <v>237.1919054268083</v>
       </c>
       <c r="D14" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15">
@@ -3211,27 +3143,27 @@
         <v>15</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>233.1179958733345</v>
+        <v>237.1919054268083</v>
       </c>
       <c r="D15" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B16" t="n">
         <v>12</v>
       </c>
       <c r="C16" t="n">
-        <v>215.7452201092761</v>
+        <v>300.273208928136</v>
       </c>
       <c r="D16" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
@@ -3239,321 +3171,321 @@
         <v>12</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C17" t="n">
-        <v>215.7452201092761</v>
+        <v>300.273208928136</v>
       </c>
       <c r="D17" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B18" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C18" t="n">
-        <v>48.66210024238575</v>
+        <v>351.7570184090148</v>
       </c>
       <c r="D18" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C19" t="n">
-        <v>48.66210024238575</v>
+        <v>351.7570184090148</v>
       </c>
       <c r="D19" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B20" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C20" t="n">
-        <v>80.95677859203639</v>
+        <v>351.9232870953555</v>
       </c>
       <c r="D20" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>80.95677859203639</v>
+        <v>351.9232870953555</v>
       </c>
       <c r="D21" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B22" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C22" t="n">
-        <v>232.4220299369231</v>
+        <v>314.4137401577736</v>
       </c>
       <c r="D22" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>232.4220299369231</v>
+        <v>314.4137401577736</v>
       </c>
       <c r="D23" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B24" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C24" t="n">
-        <v>530.7278021735813</v>
+        <v>186.2713075060139</v>
       </c>
       <c r="D24" t="n">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B25" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>530.7278021735813</v>
+        <v>186.2713075060139</v>
       </c>
       <c r="D25" t="n">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C26" t="n">
-        <v>197.8736970898356</v>
+        <v>45.5411901469428</v>
       </c>
       <c r="D26" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
+        <v>8</v>
+      </c>
+      <c r="B27" t="n">
         <v>3</v>
       </c>
-      <c r="B27" t="n">
-        <v>2</v>
-      </c>
       <c r="C27" t="n">
-        <v>197.8736970898356</v>
+        <v>45.5411901469428</v>
       </c>
       <c r="D27" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B28" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C28" t="n">
-        <v>192.3980249378876</v>
+        <v>342.4981751776205</v>
       </c>
       <c r="D28" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B29" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C29" t="n">
-        <v>192.3980249378876</v>
+        <v>342.4981751776205</v>
       </c>
       <c r="D29" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B30" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C30" t="n">
-        <v>693.9510069161944</v>
+        <v>146.6594695203825</v>
       </c>
       <c r="D30" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B31" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C31" t="n">
-        <v>693.9510069161944</v>
+        <v>146.6594695203825</v>
       </c>
       <c r="D31" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C32" t="n">
-        <v>270.0536983638625</v>
+        <v>304.8967038195067</v>
       </c>
       <c r="D32" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>270.0536983638625</v>
+        <v>304.8967038195067</v>
       </c>
       <c r="D33" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B34" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C34" t="n">
-        <v>310.7104761671225</v>
+        <v>204.8047851003487</v>
       </c>
       <c r="D34" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B35" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C35" t="n">
-        <v>310.7104761671225</v>
+        <v>204.8047851003487</v>
       </c>
       <c r="D35" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B36" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C36" t="n">
-        <v>415.7811924558397</v>
+        <v>623.0393246015857</v>
       </c>
       <c r="D36" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B37" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C37" t="n">
-        <v>415.7811924558397</v>
+        <v>623.0393246015857</v>
       </c>
       <c r="D37" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B38" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C38" t="n">
-        <v>228.3549868078208</v>
+        <v>62.96824596572466</v>
       </c>
       <c r="D38" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" t="n">
-        <v>228.3549868078208</v>
+        <v>62.96824596572466</v>
       </c>
       <c r="D39" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40">
@@ -3564,10 +3496,10 @@
         <v>10</v>
       </c>
       <c r="C40" t="n">
-        <v>274.2207140243056</v>
+        <v>109.3846424321074</v>
       </c>
       <c r="D40" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41">
@@ -3578,10 +3510,10 @@
         <v>3</v>
       </c>
       <c r="C41" t="n">
-        <v>274.2207140243056</v>
+        <v>109.3846424321074</v>
       </c>
       <c r="D41" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42">
@@ -3589,27 +3521,27 @@
         <v>2</v>
       </c>
       <c r="B42" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C42" t="n">
-        <v>116.2970334961301</v>
+        <v>66.40783086353596</v>
       </c>
       <c r="D42" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B43" t="n">
         <v>2</v>
       </c>
       <c r="C43" t="n">
-        <v>116.2970334961301</v>
+        <v>66.40783086353596</v>
       </c>
       <c r="D43" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>